<commit_message>
update Ballerup integration test
</commit_message>
<xml_diff>
--- a/tests/fixtures/BALLERUP.xlsx
+++ b/tests/fixtures/BALLERUP.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="bruger" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="300">
   <si>
     <t xml:space="preserve">operation</t>
   </si>
@@ -223,6 +223,21 @@
     <t xml:space="preserve">C</t>
   </si>
   <si>
+    <t xml:space="preserve">b4cd77e4-2ba0-47c7-93e9-22f7446abb57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noget</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tilknytning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f5b8f156-fa4e-46e2-b9e6-51a953166273</t>
+  </si>
+  <si>
     <t xml:space="preserve">brugerref_bvn</t>
   </si>
   <si>
@@ -422,9 +437,6 @@
   </si>
   <si>
     <t xml:space="preserve">2016-04-11 15:38:59.875758+02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f5b8f156-fa4e-46e2-b9e6-51a953166273</t>
   </si>
   <si>
     <t xml:space="preserve">… (≈400 flere)</t>
@@ -928,7 +940,7 @@
     <numFmt numFmtId="168" formatCode="YYYY/MM/DD"/>
     <numFmt numFmtId="169" formatCode="####"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -956,11 +968,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1074,7 +1081,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1159,10 +1166,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1199,7 +1202,7 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="L3:L54 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1208,10 +1211,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="32.68"/>
@@ -1449,17 +1452,17 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="L3:L54 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.17"/>
@@ -1544,7 +1547,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="1" sqref="L3:L54 N2"/>
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1553,7 +1556,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="4.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="2.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="31.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.85"/>
@@ -1562,7 +1565,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="12.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="1" width="32.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="1" width="32.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="8.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="17" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.83"/>
@@ -1681,15 +1684,15 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M2" activeCellId="1" sqref="L3:L54 M2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.1"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="3.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.89"/>
@@ -1698,9 +1701,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="36.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="36.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="8.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="36.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="34.93"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="256" min="14" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1758,7 +1762,7 @@
       <c r="E2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="2" t="s">
         <v>57</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -1817,6 +1821,45 @@
       </c>
       <c r="L3" s="4" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1846,7 +1889,7 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P1" activeCellId="1" sqref="L3:L54 P1"/>
+      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1861,10 +1904,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="43.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="35.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="43.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="43.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="10.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="12.85"/>
@@ -1890,63 +1933,63 @@
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B2" s="20"/>
       <c r="C2" s="16" t="n">
         <v>43115</v>
       </c>
-      <c r="D2" s="22"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="F2" s="20"/>
       <c r="G2" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>43</v>
@@ -1957,18 +2000,18 @@
       <c r="L2" s="4"/>
       <c r="M2" s="20"/>
       <c r="N2" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="O2" s="20"/>
       <c r="P2" s="4" t="s">
         <v>59</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="R2" s="20"/>
       <c r="S2" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2137,20 +2180,20 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="1" sqref="L3:L54 G2"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.39"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.46"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="3.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="37.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="37.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="8.79"/>
@@ -2158,6 +2201,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="17.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="10.01"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="253" min="16" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="254" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2177,39 +2221,39 @@
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B2" s="20"/>
       <c r="C2" s="16" t="n">
@@ -2217,7 +2261,7 @@
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="4" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F2" s="20"/>
       <c r="G2" s="4" t="s">
@@ -2241,23 +2285,23 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="23" t="n">
+      <c r="C3" s="22" t="n">
         <v>43115</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="2" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="4" t="s">
@@ -2281,15 +2325,15 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B4" s="20"/>
       <c r="C4" s="16" t="n">
@@ -2297,7 +2341,7 @@
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="4" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F4" s="20"/>
       <c r="G4" s="4" t="s">
@@ -2321,23 +2365,23 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="23" t="n">
+      <c r="C5" s="22" t="n">
         <v>43115</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="2" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="4" t="s">
@@ -2361,15 +2405,15 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="16" t="n">
@@ -2377,7 +2421,7 @@
       </c>
       <c r="D6" s="20"/>
       <c r="E6" s="4" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="F6" s="20"/>
       <c r="G6" s="4" t="s">
@@ -2401,23 +2445,23 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="23" t="n">
+      <c r="C7" s="22" t="n">
         <v>43115</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="2" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="4" t="s">
@@ -2441,15 +2485,15 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="16" t="n">
@@ -2457,9 +2501,9 @@
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F8" s="24"/>
+        <v>106</v>
+      </c>
+      <c r="F8" s="23"/>
       <c r="G8" s="4" t="s">
         <v>59</v>
       </c>
@@ -2481,25 +2525,25 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="23" t="n">
+      <c r="C9" s="22" t="n">
         <v>43115</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F9" s="25"/>
+        <v>108</v>
+      </c>
+      <c r="F9" s="24"/>
       <c r="G9" s="4" t="s">
         <v>59</v>
       </c>
@@ -2521,15 +2565,15 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B10" s="20"/>
       <c r="C10" s="16" t="n">
@@ -2537,9 +2581,9 @@
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F10" s="24"/>
+        <v>110</v>
+      </c>
+      <c r="F10" s="23"/>
       <c r="G10" s="4" t="s">
         <v>59</v>
       </c>
@@ -2561,25 +2605,25 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="23" t="n">
+      <c r="C11" s="22" t="n">
         <v>43115</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F11" s="25"/>
+        <v>112</v>
+      </c>
+      <c r="F11" s="24"/>
       <c r="G11" s="4" t="s">
         <v>59</v>
       </c>
@@ -2601,10 +2645,10 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2625,8 +2669,10 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L54" activeCellId="0" sqref="L3:L54"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="5" topLeftCell="J6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2635,29 +2681,30 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="2.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="28.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="34.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="27.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="34.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="27.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="34.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="13.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="35.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="35.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="8.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="8.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="10.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="9.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="8.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="26.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="34.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="34.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="15.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="19.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="19.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="9.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="13.82"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="255" min="27" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="256" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2677,67 +2724,67 @@
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="U1" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2746,26 +2793,26 @@
       </c>
       <c r="B2" s="20"/>
       <c r="C2" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="4" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>59</v>
@@ -2783,14 +2830,14 @@
       </c>
       <c r="O2" s="20"/>
       <c r="P2" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q2" s="4" t="str">
         <f aca="false">facet!$E$8</f>
         <v>Tilknytningstype</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S2" s="20"/>
       <c r="T2" s="20"/>
@@ -2807,26 +2854,26 @@
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="2" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>59</v>
@@ -2844,14 +2891,14 @@
       </c>
       <c r="O3" s="3"/>
       <c r="P3" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q3" s="2" t="str">
         <f aca="false">facet!$E$7</f>
         <v>Stillingsbetegnelse</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
@@ -2864,30 +2911,30 @@
     </row>
     <row r="4" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B4" s="20"/>
       <c r="C4" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="4" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H4" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>123</v>
-      </c>
       <c r="J4" s="4" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>59</v>
@@ -2905,14 +2952,14 @@
       </c>
       <c r="O4" s="20"/>
       <c r="P4" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q4" s="4" t="str">
         <f aca="false">facet!$E$7</f>
         <v>Stillingsbetegnelse</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S4" s="20"/>
       <c r="T4" s="20"/>
@@ -2925,30 +2972,30 @@
     </row>
     <row r="5" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>59</v>
@@ -2966,14 +3013,14 @@
       </c>
       <c r="O5" s="3"/>
       <c r="P5" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q5" s="2" t="str">
         <f aca="false">facet!$E$7</f>
         <v>Stillingsbetegnelse</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
@@ -2986,30 +3033,30 @@
     </row>
     <row r="6" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>132</v>
+        <v>69</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D6" s="20"/>
       <c r="E6" s="4" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>59</v>
@@ -3027,14 +3074,14 @@
       </c>
       <c r="O6" s="20"/>
       <c r="P6" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q6" s="4" t="str">
         <f aca="false">facet!$E$7</f>
         <v>Stillingsbetegnelse</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S6" s="20"/>
       <c r="T6" s="20"/>
@@ -3047,30 +3094,30 @@
     </row>
     <row r="7" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="2" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>59</v>
@@ -3088,14 +3135,14 @@
       </c>
       <c r="O7" s="3"/>
       <c r="P7" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q7" s="2" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
@@ -3108,30 +3155,30 @@
     </row>
     <row r="8" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="4" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>59</v>
@@ -3149,14 +3196,14 @@
       </c>
       <c r="O8" s="20"/>
       <c r="P8" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q8" s="4" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S8" s="20"/>
       <c r="T8" s="20"/>
@@ -3169,27 +3216,27 @@
     </row>
     <row r="9" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>31</v>
@@ -3210,18 +3257,18 @@
       </c>
       <c r="O9" s="3"/>
       <c r="P9" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q9" s="2" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S9" s="3"/>
       <c r="T9" s="2" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
@@ -3232,30 +3279,30 @@
     </row>
     <row r="10" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B10" s="20"/>
       <c r="C10" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="4" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>59</v>
@@ -3273,14 +3320,14 @@
       </c>
       <c r="O10" s="20"/>
       <c r="P10" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q10" s="4" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S10" s="20"/>
       <c r="T10" s="20"/>
@@ -3293,30 +3340,30 @@
     </row>
     <row r="11" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="2" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>59</v>
@@ -3334,14 +3381,14 @@
       </c>
       <c r="O11" s="3"/>
       <c r="P11" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q11" s="2" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
@@ -3354,30 +3401,30 @@
     </row>
     <row r="12" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B12" s="20"/>
       <c r="C12" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="4" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>59</v>
@@ -3395,14 +3442,14 @@
       </c>
       <c r="O12" s="20"/>
       <c r="P12" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q12" s="4" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S12" s="20"/>
       <c r="T12" s="20"/>
@@ -3415,30 +3462,30 @@
     </row>
     <row r="13" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>59</v>
@@ -3456,14 +3503,14 @@
       </c>
       <c r="O13" s="3"/>
       <c r="P13" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q13" s="2" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
@@ -3476,30 +3523,30 @@
     </row>
     <row r="14" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="B14" s="20"/>
       <c r="C14" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="4" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>59</v>
@@ -3517,14 +3564,14 @@
       </c>
       <c r="O14" s="20"/>
       <c r="P14" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q14" s="4" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S14" s="20"/>
       <c r="T14" s="20"/>
@@ -3537,30 +3584,30 @@
     </row>
     <row r="15" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="2" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>59</v>
@@ -3578,14 +3625,14 @@
       </c>
       <c r="O15" s="3"/>
       <c r="P15" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q15" s="2" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
@@ -3598,30 +3645,30 @@
     </row>
     <row r="16" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B16" s="20"/>
       <c r="C16" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="4" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>59</v>
@@ -3639,14 +3686,14 @@
       </c>
       <c r="O16" s="20"/>
       <c r="P16" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q16" s="4" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S16" s="20"/>
       <c r="T16" s="20"/>
@@ -3659,30 +3706,30 @@
     </row>
     <row r="17" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="2" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>59</v>
@@ -3700,14 +3747,14 @@
       </c>
       <c r="O17" s="3"/>
       <c r="P17" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q17" s="2" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
@@ -3720,30 +3767,30 @@
     </row>
     <row r="18" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B18" s="20"/>
       <c r="C18" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="4" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>59</v>
@@ -3761,14 +3808,14 @@
       </c>
       <c r="O18" s="20"/>
       <c r="P18" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q18" s="4" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R18" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S18" s="20"/>
       <c r="T18" s="20"/>
@@ -3781,30 +3828,30 @@
     </row>
     <row r="19" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="2" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>59</v>
@@ -3822,14 +3869,14 @@
       </c>
       <c r="O19" s="3"/>
       <c r="P19" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q19" s="2" t="str">
         <f aca="false">facet!$E$9</f>
         <v>Ledertyper</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
@@ -3842,30 +3889,30 @@
     </row>
     <row r="20" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B20" s="20"/>
       <c r="C20" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="4" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="K20" s="4" t="s">
         <v>59</v>
@@ -3883,14 +3930,14 @@
       </c>
       <c r="O20" s="20"/>
       <c r="P20" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q20" s="4" t="str">
         <f aca="false">facet!$E$9</f>
         <v>Ledertyper</v>
       </c>
       <c r="R20" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S20" s="20"/>
       <c r="T20" s="20"/>
@@ -3903,30 +3950,30 @@
     </row>
     <row r="21" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="2" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="K21" s="4" t="s">
         <v>59</v>
@@ -3944,14 +3991,14 @@
       </c>
       <c r="O21" s="3"/>
       <c r="P21" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q21" s="2" t="str">
         <f aca="false">facet!$E$9</f>
         <v>Ledertyper</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
@@ -3964,30 +4011,30 @@
     </row>
     <row r="22" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B22" s="20"/>
       <c r="C22" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="4" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="K22" s="4" t="s">
         <v>59</v>
@@ -4005,14 +4052,14 @@
       </c>
       <c r="O22" s="20"/>
       <c r="P22" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q22" s="4" t="str">
         <f aca="false">facet!$E$9</f>
         <v>Ledertyper</v>
       </c>
       <c r="R22" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S22" s="20"/>
       <c r="T22" s="20"/>
@@ -4025,30 +4072,30 @@
     </row>
     <row r="23" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="2" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="K23" s="4" t="s">
         <v>59</v>
@@ -4066,14 +4113,14 @@
       </c>
       <c r="O23" s="3"/>
       <c r="P23" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q23" s="2" t="str">
         <f aca="false">facet!$E$9</f>
         <v>Ledertyper</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
@@ -4086,30 +4133,30 @@
     </row>
     <row r="24" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B24" s="20"/>
       <c r="C24" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="4" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="K24" s="4" t="s">
         <v>59</v>
@@ -4127,14 +4174,14 @@
       </c>
       <c r="O24" s="20"/>
       <c r="P24" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q24" s="4" t="str">
         <f aca="false">facet!$E$9</f>
         <v>Ledertyper</v>
       </c>
       <c r="R24" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S24" s="20"/>
       <c r="T24" s="20"/>
@@ -4147,30 +4194,30 @@
     </row>
     <row r="25" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="2" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="K25" s="4" t="s">
         <v>59</v>
@@ -4188,14 +4235,14 @@
       </c>
       <c r="O25" s="3"/>
       <c r="P25" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q25" s="2" t="str">
         <f aca="false">facet!$E$9</f>
         <v>Ledertyper</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
@@ -4208,30 +4255,30 @@
     </row>
     <row r="26" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B26" s="20"/>
       <c r="C26" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="4" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="K26" s="4" t="s">
         <v>59</v>
@@ -4249,14 +4296,14 @@
       </c>
       <c r="O26" s="20"/>
       <c r="P26" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q26" s="4" t="str">
         <f aca="false">facet!$E$9</f>
         <v>Ledertyper</v>
       </c>
       <c r="R26" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S26" s="20"/>
       <c r="T26" s="20"/>
@@ -4269,30 +4316,30 @@
     </row>
     <row r="27" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="2" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="K27" s="4" t="s">
         <v>59</v>
@@ -4310,14 +4357,14 @@
       </c>
       <c r="O27" s="3"/>
       <c r="P27" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q27" s="2" t="str">
         <f aca="false">facet!$E$9</f>
         <v>Ledertyper</v>
       </c>
       <c r="R27" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
@@ -4330,30 +4377,30 @@
     </row>
     <row r="28" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B28" s="20"/>
       <c r="C28" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="4" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="K28" s="4" t="s">
         <v>59</v>
@@ -4371,14 +4418,14 @@
       </c>
       <c r="O28" s="20"/>
       <c r="P28" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q28" s="4" t="str">
         <f aca="false">facet!$E$9</f>
         <v>Ledertyper</v>
       </c>
       <c r="R28" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S28" s="20"/>
       <c r="T28" s="20"/>
@@ -4391,30 +4438,30 @@
     </row>
     <row r="29" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="2" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="K29" s="4" t="s">
         <v>59</v>
@@ -4432,14 +4479,14 @@
       </c>
       <c r="O29" s="3"/>
       <c r="P29" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q29" s="2" t="str">
         <f aca="false">facet!$E$9</f>
         <v>Ledertyper</v>
       </c>
       <c r="R29" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
@@ -4452,30 +4499,30 @@
     </row>
     <row r="30" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B30" s="20"/>
       <c r="C30" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D30" s="20"/>
       <c r="E30" s="4" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="K30" s="4" t="s">
         <v>59</v>
@@ -4493,14 +4540,14 @@
       </c>
       <c r="O30" s="20"/>
       <c r="P30" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q30" s="4" t="str">
         <f aca="false">facet!$E$9</f>
         <v>Ledertyper</v>
       </c>
       <c r="R30" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S30" s="20"/>
       <c r="T30" s="20"/>
@@ -4513,30 +4560,30 @@
     </row>
     <row r="31" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="2" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="K31" s="4" t="s">
         <v>59</v>
@@ -4554,14 +4601,14 @@
       </c>
       <c r="O31" s="3"/>
       <c r="P31" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q31" s="2" t="str">
         <f aca="false">facet!$E$9</f>
         <v>Ledertyper</v>
       </c>
       <c r="R31" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
@@ -4574,30 +4621,30 @@
     </row>
     <row r="32" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B32" s="20"/>
       <c r="C32" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D32" s="20"/>
       <c r="E32" s="4" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="K32" s="4" t="s">
         <v>59</v>
@@ -4615,14 +4662,14 @@
       </c>
       <c r="O32" s="20"/>
       <c r="P32" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q32" s="4" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Lederansvar</v>
       </c>
       <c r="R32" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S32" s="20"/>
       <c r="T32" s="20"/>
@@ -4635,30 +4682,30 @@
     </row>
     <row r="33" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="2" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="K33" s="4" t="s">
         <v>59</v>
@@ -4676,14 +4723,14 @@
       </c>
       <c r="O33" s="3"/>
       <c r="P33" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q33" s="2" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Lederansvar</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
@@ -4696,30 +4743,30 @@
     </row>
     <row r="34" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="B34" s="20"/>
       <c r="C34" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D34" s="20"/>
       <c r="E34" s="4" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="K34" s="4" t="s">
         <v>59</v>
@@ -4737,14 +4784,14 @@
       </c>
       <c r="O34" s="20"/>
       <c r="P34" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q34" s="4" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Lederansvar</v>
       </c>
       <c r="R34" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S34" s="20"/>
       <c r="T34" s="20"/>
@@ -4757,30 +4804,30 @@
     </row>
     <row r="35" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="2" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="K35" s="4" t="s">
         <v>59</v>
@@ -4798,14 +4845,14 @@
       </c>
       <c r="O35" s="3"/>
       <c r="P35" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q35" s="2" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Lederansvar</v>
       </c>
       <c r="R35" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
@@ -4818,30 +4865,30 @@
     </row>
     <row r="36" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B36" s="20"/>
       <c r="C36" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D36" s="20"/>
       <c r="E36" s="4" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="K36" s="4" t="s">
         <v>59</v>
@@ -4859,14 +4906,14 @@
       </c>
       <c r="O36" s="20"/>
       <c r="P36" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q36" s="4" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Lederansvar</v>
       </c>
       <c r="R36" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S36" s="20"/>
       <c r="T36" s="20"/>
@@ -4879,30 +4926,30 @@
     </row>
     <row r="37" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="2" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="K37" s="4" t="s">
         <v>59</v>
@@ -4920,14 +4967,14 @@
       </c>
       <c r="O37" s="3"/>
       <c r="P37" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q37" s="2" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Lederansvar</v>
       </c>
       <c r="R37" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
@@ -4940,30 +4987,30 @@
     </row>
     <row r="38" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="B38" s="20"/>
       <c r="C38" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D38" s="20"/>
       <c r="E38" s="4" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="K38" s="4" t="s">
         <v>59</v>
@@ -4981,14 +5028,14 @@
       </c>
       <c r="O38" s="20"/>
       <c r="P38" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q38" s="4" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Lederansvar</v>
       </c>
       <c r="R38" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S38" s="20"/>
       <c r="T38" s="20"/>
@@ -5001,30 +5048,30 @@
     </row>
     <row r="39" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="2" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="K39" s="4" t="s">
         <v>59</v>
@@ -5042,14 +5089,14 @@
       </c>
       <c r="O39" s="3"/>
       <c r="P39" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q39" s="2" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Lederansvar</v>
       </c>
       <c r="R39" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
@@ -5062,30 +5109,30 @@
     </row>
     <row r="40" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B40" s="20"/>
       <c r="C40" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D40" s="20"/>
       <c r="E40" s="4" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="K40" s="4" t="s">
         <v>59</v>
@@ -5103,14 +5150,14 @@
       </c>
       <c r="O40" s="20"/>
       <c r="P40" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q40" s="4" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Lederansvar</v>
       </c>
       <c r="R40" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S40" s="20"/>
       <c r="T40" s="20"/>
@@ -5123,30 +5170,30 @@
     </row>
     <row r="41" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="2" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>59</v>
@@ -5164,14 +5211,14 @@
       </c>
       <c r="O41" s="3"/>
       <c r="P41" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q41" s="2" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Lederansvar</v>
       </c>
       <c r="R41" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
@@ -5184,30 +5231,30 @@
     </row>
     <row r="42" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B42" s="20"/>
       <c r="C42" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="4" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>59</v>
@@ -5225,21 +5272,21 @@
       </c>
       <c r="O42" s="20"/>
       <c r="P42" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q42" s="4" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Adressetype</v>
       </c>
       <c r="R42" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S42" s="4" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="T42" s="20"/>
       <c r="U42" s="4" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="V42" s="20"/>
       <c r="W42" s="20"/>
@@ -5249,30 +5296,30 @@
     </row>
     <row r="43" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="2" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>59</v>
@@ -5290,21 +5337,21 @@
       </c>
       <c r="O43" s="3"/>
       <c r="P43" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q43" s="2" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Adressetype</v>
       </c>
       <c r="R43" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S43" s="2" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="T43" s="3"/>
       <c r="U43" s="2" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="V43" s="3"/>
       <c r="W43" s="3"/>
@@ -5314,30 +5361,30 @@
     </row>
     <row r="44" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="B44" s="20"/>
       <c r="C44" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="4" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="K44" s="4" t="s">
         <v>59</v>
@@ -5355,17 +5402,17 @@
       </c>
       <c r="O44" s="20"/>
       <c r="P44" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q44" s="4" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Adressetype</v>
       </c>
       <c r="R44" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S44" s="4" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="T44" s="20"/>
       <c r="U44" s="20"/>
@@ -5377,30 +5424,30 @@
     </row>
     <row r="45" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="B45" s="3"/>
       <c r="C45" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="2" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="K45" s="4" t="s">
         <v>59</v>
@@ -5418,17 +5465,17 @@
       </c>
       <c r="O45" s="3"/>
       <c r="P45" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q45" s="2" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Adressetype</v>
       </c>
       <c r="R45" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S45" s="2" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="T45" s="3"/>
       <c r="U45" s="3"/>
@@ -5440,30 +5487,30 @@
     </row>
     <row r="46" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="B46" s="20"/>
       <c r="C46" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="4" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="K46" s="4" t="s">
         <v>59</v>
@@ -5481,21 +5528,21 @@
       </c>
       <c r="O46" s="20"/>
       <c r="P46" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q46" s="4" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Adressetype</v>
       </c>
       <c r="R46" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S46" s="4" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="T46" s="20"/>
       <c r="U46" s="4" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="V46" s="20"/>
       <c r="W46" s="20"/>
@@ -5505,22 +5552,22 @@
     </row>
     <row r="47" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="2" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
       <c r="J47" s="2" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="K47" s="4" t="s">
         <v>59</v>
@@ -5538,21 +5585,21 @@
       </c>
       <c r="O47" s="3"/>
       <c r="P47" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q47" s="2" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Adressetype</v>
       </c>
       <c r="R47" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S47" s="2" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="T47" s="3"/>
       <c r="U47" s="2" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="V47" s="3"/>
       <c r="W47" s="3"/>
@@ -5562,22 +5609,22 @@
     </row>
     <row r="48" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="B48" s="20"/>
       <c r="C48" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="4" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="F48" s="20"/>
       <c r="G48" s="20"/>
       <c r="H48" s="20"/>
       <c r="I48" s="20"/>
       <c r="J48" s="4" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="K48" s="4" t="s">
         <v>59</v>
@@ -5595,21 +5642,21 @@
       </c>
       <c r="O48" s="20"/>
       <c r="P48" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q48" s="4" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Adressetype</v>
       </c>
       <c r="R48" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S48" s="4" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="T48" s="20"/>
       <c r="U48" s="4" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="V48" s="20"/>
       <c r="W48" s="20"/>
@@ -5619,22 +5666,22 @@
     </row>
     <row r="49" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="2" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
       <c r="J49" s="2" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="K49" s="4" t="s">
         <v>59</v>
@@ -5652,21 +5699,21 @@
       </c>
       <c r="O49" s="3"/>
       <c r="P49" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q49" s="2" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Adressetype</v>
       </c>
       <c r="R49" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S49" s="2" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="T49" s="3"/>
       <c r="U49" s="2" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="V49" s="3"/>
       <c r="W49" s="3"/>
@@ -5676,22 +5723,22 @@
     </row>
     <row r="50" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="B50" s="20"/>
       <c r="C50" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D50" s="20"/>
       <c r="E50" s="4" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="F50" s="20"/>
       <c r="G50" s="20"/>
       <c r="H50" s="20"/>
       <c r="I50" s="20"/>
       <c r="J50" s="4" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="K50" s="4" t="s">
         <v>59</v>
@@ -5709,21 +5756,21 @@
       </c>
       <c r="O50" s="20"/>
       <c r="P50" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q50" s="4" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Adressetype</v>
       </c>
       <c r="R50" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S50" s="4" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="T50" s="20"/>
       <c r="U50" s="4" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="V50" s="20"/>
       <c r="W50" s="20"/>
@@ -5733,22 +5780,22 @@
     </row>
     <row r="51" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="B51" s="3"/>
       <c r="C51" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="2" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
       <c r="J51" s="2" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="K51" s="4" t="s">
         <v>59</v>
@@ -5766,17 +5813,17 @@
       </c>
       <c r="O51" s="3"/>
       <c r="P51" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q51" s="2" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Adressetype</v>
       </c>
       <c r="R51" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S51" s="2" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="T51" s="3"/>
       <c r="U51" s="3" t="n">
@@ -5790,22 +5837,22 @@
     </row>
     <row r="52" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B52" s="20"/>
       <c r="C52" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D52" s="20"/>
       <c r="E52" s="4" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="F52" s="20"/>
       <c r="G52" s="20"/>
       <c r="H52" s="20"/>
       <c r="I52" s="20"/>
       <c r="J52" s="4" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="K52" s="4" t="s">
         <v>59</v>
@@ -5823,21 +5870,21 @@
       </c>
       <c r="O52" s="20"/>
       <c r="P52" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q52" s="4" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Adressetype</v>
       </c>
       <c r="R52" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S52" s="4" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="T52" s="20"/>
       <c r="U52" s="4" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="V52" s="20"/>
       <c r="W52" s="20"/>
@@ -5847,22 +5894,22 @@
     </row>
     <row r="53" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="2" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
       <c r="J53" s="2" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="K53" s="4" t="s">
         <v>59</v>
@@ -5880,21 +5927,21 @@
       </c>
       <c r="O53" s="3"/>
       <c r="P53" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q53" s="2" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Adressetype</v>
       </c>
       <c r="R53" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S53" s="2" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="T53" s="3"/>
       <c r="U53" s="2" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="V53" s="3"/>
       <c r="W53" s="3"/>
@@ -5904,22 +5951,22 @@
     </row>
     <row r="54" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="B54" s="20"/>
       <c r="C54" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D54" s="20"/>
       <c r="E54" s="4" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="F54" s="20"/>
       <c r="G54" s="20"/>
       <c r="H54" s="20"/>
       <c r="I54" s="20"/>
       <c r="J54" s="4" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="K54" s="4" t="s">
         <v>59</v>
@@ -5937,21 +5984,21 @@
       </c>
       <c r="O54" s="20"/>
       <c r="P54" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q54" s="4" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Adressetype</v>
       </c>
       <c r="R54" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S54" s="4" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="T54" s="20"/>
       <c r="U54" s="4" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="V54" s="20"/>
       <c r="W54" s="20"/>

</xml_diff>

<commit_message>
Added role and leave data to BALLERUP.xlsx
</commit_message>
<xml_diff>
--- a/tests/fixtures/BALLERUP.xlsx
+++ b/tests/fixtures/BALLERUP.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="bruger" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="315">
   <si>
     <t xml:space="preserve">operation</t>
   </si>
@@ -236,6 +236,30 @@
   </si>
   <si>
     <t xml:space="preserve">f5b8f156-fa4e-46e2-b9e6-51a953166273</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3b204d9b-a0ba-48ad-9c20-778a49b6d3a9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rolle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d82de46c-e266-4810-9e8d-e99a0c9c18d5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orlov</t>
   </si>
   <si>
     <t xml:space="preserve">brugerref_bvn</t>
@@ -965,7 +989,7 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -987,14 +1011,14 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1231,29 +1255,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M1048576"/>
+  <dimension ref="A1:M65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15.4"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="32.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="8.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="15.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="14" style="1" width="8.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.83"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.24696356275304"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="4.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="6.10526315789474"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="32.8866396761134"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.24696356275304"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="256" min="14" style="1" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1468,7 +1492,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1483,23 +1507,23 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15.4"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="10" style="1" width="8.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.83"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.10526315789474"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.24696356275304"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="256" min="10" style="1" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1563,7 +1587,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
@@ -1578,29 +1602,29 @@
   </sheetPr>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15.4"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="4.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="2.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="31.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="12.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="1" width="32.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="8.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="17" style="1" width="8.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.83"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="4.17813765182186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="2.25101214574899"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.9271255060729"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.497975708502"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.24696356275304"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="1" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="8.24696356275304"/>
+    <col collapsed="false" hidden="false" max="256" min="17" style="1" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1701,7 +1725,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
@@ -1714,29 +1738,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M1048576"/>
+  <dimension ref="A1:M65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15.4"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="3.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="36.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="27.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="36.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="36.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="34.93"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="256" min="14" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.1417004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.4615384615385"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="3.10526315789474"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.9271255060729"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="36.6356275303644"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="36.9554655870445"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="36.9554655870445"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="35.1336032388664"/>
+    <col collapsed="false" hidden="false" max="256" min="14" style="1" width="11.5708502024291"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1854,6 +1878,7 @@
       <c r="L3" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="M3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
@@ -1893,6 +1918,78 @@
       <c r="M4" s="4" t="s">
         <v>69</v>
       </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
     </row>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1905,7 +2002,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1920,32 +2017,32 @@
   </sheetPr>
   <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15.4"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="43.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="34.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="43.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="35.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="17.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="43.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="43.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="12.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="20" style="1" width="8.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.83"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.96356275303644"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.497975708502"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="34.4939271255061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="43.919028340081"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="35.4574898785425"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="43.919028340081"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="43.919028340081"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="10.497975708502"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="256" min="20" style="1" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1965,51 +2062,51 @@
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B2" s="20"/>
       <c r="C2" s="16" t="n">
@@ -2017,11 +2114,11 @@
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="4" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="F2" s="20"/>
       <c r="G2" s="4" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>43</v>
@@ -2032,18 +2129,18 @@
       <c r="L2" s="4"/>
       <c r="M2" s="20"/>
       <c r="N2" s="4" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="O2" s="20"/>
       <c r="P2" s="4" t="s">
         <v>59</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="R2" s="20"/>
       <c r="S2" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2196,7 +2293,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.3"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
@@ -2211,29 +2308,29 @@
   </sheetPr>
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15.4"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.39"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="3.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="37.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="37.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="36.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="17.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="10.01"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="253" min="16" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="254" style="0" width="8.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="38.0283400809717"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.46153846153846"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.4615384615385"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="3.10526315789474"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.9271255060729"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.6032388663968"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="37.919028340081"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.1052631578947"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="37.919028340081"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="36.9554655870445"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="253" min="16" style="1" width="11.5708502024291"/>
+    <col collapsed="false" hidden="false" max="1025" min="254" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2253,39 +2350,39 @@
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B2" s="20"/>
       <c r="C2" s="16" t="n">
@@ -2293,7 +2390,7 @@
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="4" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F2" s="20"/>
       <c r="G2" s="4" t="s">
@@ -2317,15 +2414,15 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="22" t="n">
@@ -2333,7 +2430,7 @@
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="2" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="4" t="s">
@@ -2357,15 +2454,15 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B4" s="20"/>
       <c r="C4" s="16" t="n">
@@ -2373,7 +2470,7 @@
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="4" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="F4" s="20"/>
       <c r="G4" s="4" t="s">
@@ -2397,15 +2494,15 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="22" t="n">
@@ -2413,7 +2510,7 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="2" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="4" t="s">
@@ -2437,15 +2534,15 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="16" t="n">
@@ -2453,7 +2550,7 @@
       </c>
       <c r="D6" s="20"/>
       <c r="E6" s="4" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="F6" s="20"/>
       <c r="G6" s="4" t="s">
@@ -2477,15 +2574,15 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="22" t="n">
@@ -2493,7 +2590,7 @@
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="2" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="4" t="s">
@@ -2517,15 +2614,15 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="16" t="n">
@@ -2533,7 +2630,7 @@
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="4" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="4" t="s">
@@ -2557,15 +2654,15 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="24" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="16" t="n">
@@ -2573,7 +2670,7 @@
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="24" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="4" t="s">
@@ -2597,15 +2694,15 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="22" t="n">
@@ -2613,7 +2710,7 @@
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="2" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="F10" s="25"/>
       <c r="G10" s="4" t="s">
@@ -2637,15 +2734,15 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="16" t="n">
@@ -2653,7 +2750,7 @@
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="4" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="4" t="s">
@@ -2677,15 +2774,15 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="22" t="n">
@@ -2693,7 +2790,7 @@
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="2" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="4" t="s">
@@ -2717,16 +2814,16 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.3"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
@@ -2741,42 +2838,42 @@
   </sheetPr>
   <dimension ref="A1:Z57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="5" topLeftCell="J6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15.4"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="2.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="28.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="34.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="27.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="34.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="13.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="35.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="35.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="8.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="10.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="9.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="8.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="26.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="34.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="15.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="19.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="13.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="9.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="13.82"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="255" min="27" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="256" style="0" width="8.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="36.2064777327935"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.1417004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="3"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="34.3846153846154"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="28.3846153846154"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="34.8137651821862"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="27.9595141700405"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="34.3846153846154"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="35.4574898785425"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="11.246963562753"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="35.4574898785425"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="8.46153846153846"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="9.63967611336032"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="8.67611336032389"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="26.8866396761134"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="34.7085020242915"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="13.8178137651822"/>
+    <col collapsed="false" hidden="false" max="255" min="27" style="1" width="11.5708502024291"/>
+    <col collapsed="false" hidden="false" max="1025" min="256" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2796,67 +2893,67 @@
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2865,26 +2962,26 @@
       </c>
       <c r="B2" s="20"/>
       <c r="C2" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="4" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>59</v>
@@ -2902,14 +2999,14 @@
       </c>
       <c r="O2" s="20"/>
       <c r="P2" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q2" s="4" t="str">
         <f aca="false">facet!$E$8</f>
         <v>Tilknytningstype</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S2" s="20"/>
       <c r="T2" s="20"/>
@@ -2922,30 +3019,30 @@
     </row>
     <row r="3" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="24" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B3" s="20"/>
       <c r="C3" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D3" s="20"/>
       <c r="E3" s="4" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>59</v>
@@ -2963,13 +3060,13 @@
       </c>
       <c r="O3" s="20"/>
       <c r="P3" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S3" s="20"/>
       <c r="T3" s="20"/>
@@ -2982,30 +3079,30 @@
     </row>
     <row r="4" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="B4" s="20"/>
       <c r="C4" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="4" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>59</v>
@@ -3023,13 +3120,13 @@
       </c>
       <c r="O4" s="20"/>
       <c r="P4" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S4" s="20"/>
       <c r="T4" s="20"/>
@@ -3042,30 +3139,30 @@
     </row>
     <row r="5" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="24" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D5" s="20"/>
       <c r="E5" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>127</v>
-      </c>
       <c r="G5" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>59</v>
@@ -3083,13 +3180,13 @@
       </c>
       <c r="O5" s="20"/>
       <c r="P5" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S5" s="20"/>
       <c r="T5" s="20"/>
@@ -3106,26 +3203,26 @@
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="H6" s="2" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>59</v>
@@ -3143,14 +3240,14 @@
       </c>
       <c r="O6" s="3"/>
       <c r="P6" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q6" s="2" t="str">
         <f aca="false">facet!$E$7</f>
         <v>Stillingsbetegnelse</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
@@ -3163,30 +3260,30 @@
     </row>
     <row r="7" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="4" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>59</v>
@@ -3204,14 +3301,14 @@
       </c>
       <c r="O7" s="20"/>
       <c r="P7" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q7" s="4" t="str">
         <f aca="false">facet!$E$7</f>
         <v>Stillingsbetegnelse</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S7" s="20"/>
       <c r="T7" s="20"/>
@@ -3224,30 +3321,30 @@
     </row>
     <row r="8" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="2" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>59</v>
@@ -3265,14 +3362,14 @@
       </c>
       <c r="O8" s="3"/>
       <c r="P8" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q8" s="2" t="str">
         <f aca="false">facet!$E$7</f>
         <v>Stillingsbetegnelse</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
@@ -3289,26 +3386,26 @@
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="4" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>59</v>
@@ -3326,14 +3423,14 @@
       </c>
       <c r="O9" s="20"/>
       <c r="P9" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q9" s="4" t="str">
         <f aca="false">facet!$E$7</f>
         <v>Stillingsbetegnelse</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S9" s="20"/>
       <c r="T9" s="20"/>
@@ -3346,30 +3443,30 @@
     </row>
     <row r="10" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="2" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>59</v>
@@ -3387,14 +3484,14 @@
       </c>
       <c r="O10" s="3"/>
       <c r="P10" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q10" s="2" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
@@ -3407,30 +3504,30 @@
     </row>
     <row r="11" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="4" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>59</v>
@@ -3448,14 +3545,14 @@
       </c>
       <c r="O11" s="20"/>
       <c r="P11" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q11" s="4" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S11" s="20"/>
       <c r="T11" s="20"/>
@@ -3468,27 +3565,27 @@
     </row>
     <row r="12" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>31</v>
@@ -3509,18 +3606,18 @@
       </c>
       <c r="O12" s="3"/>
       <c r="P12" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q12" s="2" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S12" s="3"/>
       <c r="T12" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
@@ -3531,30 +3628,30 @@
     </row>
     <row r="13" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="B13" s="20"/>
       <c r="C13" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="4" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>59</v>
@@ -3572,14 +3669,14 @@
       </c>
       <c r="O13" s="20"/>
       <c r="P13" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q13" s="4" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S13" s="20"/>
       <c r="T13" s="20"/>
@@ -3592,30 +3689,30 @@
     </row>
     <row r="14" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="2" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>59</v>
@@ -3633,14 +3730,14 @@
       </c>
       <c r="O14" s="3"/>
       <c r="P14" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q14" s="2" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
@@ -3653,30 +3750,30 @@
     </row>
     <row r="15" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="B15" s="20"/>
       <c r="C15" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="4" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>59</v>
@@ -3694,14 +3791,14 @@
       </c>
       <c r="O15" s="20"/>
       <c r="P15" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q15" s="4" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S15" s="20"/>
       <c r="T15" s="20"/>
@@ -3714,30 +3811,30 @@
     </row>
     <row r="16" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="2" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>59</v>
@@ -3755,14 +3852,14 @@
       </c>
       <c r="O16" s="3"/>
       <c r="P16" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q16" s="2" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
@@ -3775,30 +3872,30 @@
     </row>
     <row r="17" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="B17" s="20"/>
       <c r="C17" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="4" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>59</v>
@@ -3816,14 +3913,14 @@
       </c>
       <c r="O17" s="20"/>
       <c r="P17" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q17" s="4" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R17" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S17" s="20"/>
       <c r="T17" s="20"/>
@@ -3836,30 +3933,30 @@
     </row>
     <row r="18" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="2" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>59</v>
@@ -3877,14 +3974,14 @@
       </c>
       <c r="O18" s="3"/>
       <c r="P18" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q18" s="2" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
@@ -3897,30 +3994,30 @@
     </row>
     <row r="19" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="B19" s="20"/>
       <c r="C19" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="4" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>59</v>
@@ -3938,14 +4035,14 @@
       </c>
       <c r="O19" s="20"/>
       <c r="P19" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q19" s="4" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R19" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S19" s="20"/>
       <c r="T19" s="20"/>
@@ -3958,30 +4055,30 @@
     </row>
     <row r="20" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="2" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="K20" s="4" t="s">
         <v>59</v>
@@ -3999,14 +4096,14 @@
       </c>
       <c r="O20" s="3"/>
       <c r="P20" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q20" s="2" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
@@ -4019,30 +4116,30 @@
     </row>
     <row r="21" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B21" s="20"/>
       <c r="C21" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="4" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="K21" s="4" t="s">
         <v>59</v>
@@ -4060,14 +4157,14 @@
       </c>
       <c r="O21" s="20"/>
       <c r="P21" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q21" s="4" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R21" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S21" s="20"/>
       <c r="T21" s="20"/>
@@ -4080,30 +4177,30 @@
     </row>
     <row r="22" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="2" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="K22" s="4" t="s">
         <v>59</v>
@@ -4121,14 +4218,14 @@
       </c>
       <c r="O22" s="3"/>
       <c r="P22" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q22" s="2" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
@@ -4141,30 +4238,30 @@
     </row>
     <row r="23" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="B23" s="20"/>
       <c r="C23" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="4" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="K23" s="4" t="s">
         <v>59</v>
@@ -4182,14 +4279,14 @@
       </c>
       <c r="O23" s="20"/>
       <c r="P23" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q23" s="4" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R23" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S23" s="20"/>
       <c r="T23" s="20"/>
@@ -4202,30 +4299,30 @@
     </row>
     <row r="24" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="K24" s="4" t="s">
         <v>59</v>
@@ -4243,14 +4340,14 @@
       </c>
       <c r="O24" s="3"/>
       <c r="P24" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q24" s="2" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
@@ -4263,30 +4360,30 @@
     </row>
     <row r="25" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="B25" s="20"/>
       <c r="C25" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="4" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="K25" s="4" t="s">
         <v>59</v>
@@ -4304,14 +4401,14 @@
       </c>
       <c r="O25" s="20"/>
       <c r="P25" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q25" s="4" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R25" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S25" s="20"/>
       <c r="T25" s="20"/>
@@ -4324,30 +4421,30 @@
     </row>
     <row r="26" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="2" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="K26" s="4" t="s">
         <v>59</v>
@@ -4365,14 +4462,14 @@
       </c>
       <c r="O26" s="3"/>
       <c r="P26" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q26" s="2" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
@@ -4385,30 +4482,30 @@
     </row>
     <row r="27" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="B27" s="20"/>
       <c r="C27" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="4" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="K27" s="4" t="s">
         <v>59</v>
@@ -4426,14 +4523,14 @@
       </c>
       <c r="O27" s="20"/>
       <c r="P27" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q27" s="4" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R27" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S27" s="20"/>
       <c r="T27" s="20"/>
@@ -4446,30 +4543,30 @@
     </row>
     <row r="28" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="2" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="K28" s="4" t="s">
         <v>59</v>
@@ -4487,14 +4584,14 @@
       </c>
       <c r="O28" s="3"/>
       <c r="P28" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q28" s="2" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
@@ -4507,30 +4604,30 @@
     </row>
     <row r="29" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="B29" s="20"/>
       <c r="C29" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="4" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="K29" s="4" t="s">
         <v>59</v>
@@ -4548,14 +4645,14 @@
       </c>
       <c r="O29" s="20"/>
       <c r="P29" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q29" s="4" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R29" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S29" s="20"/>
       <c r="T29" s="20"/>
@@ -4568,30 +4665,30 @@
     </row>
     <row r="30" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="2" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="K30" s="4" t="s">
         <v>59</v>
@@ -4609,14 +4706,14 @@
       </c>
       <c r="O30" s="3"/>
       <c r="P30" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q30" s="2" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R30" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
@@ -4629,30 +4726,30 @@
     </row>
     <row r="31" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="B31" s="20"/>
       <c r="C31" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D31" s="20"/>
       <c r="E31" s="4" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="K31" s="4" t="s">
         <v>59</v>
@@ -4670,14 +4767,14 @@
       </c>
       <c r="O31" s="20"/>
       <c r="P31" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q31" s="4" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R31" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S31" s="20"/>
       <c r="T31" s="20"/>
@@ -4690,30 +4787,30 @@
     </row>
     <row r="32" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="2" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="K32" s="4" t="s">
         <v>59</v>
@@ -4731,14 +4828,14 @@
       </c>
       <c r="O32" s="3"/>
       <c r="P32" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q32" s="2" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
@@ -4751,30 +4848,30 @@
     </row>
     <row r="33" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="B33" s="20"/>
       <c r="C33" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D33" s="20"/>
       <c r="E33" s="4" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="K33" s="4" t="s">
         <v>59</v>
@@ -4792,14 +4889,14 @@
       </c>
       <c r="O33" s="20"/>
       <c r="P33" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q33" s="4" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R33" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S33" s="20"/>
       <c r="T33" s="20"/>
@@ -4812,30 +4909,30 @@
     </row>
     <row r="34" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="2" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="K34" s="4" t="s">
         <v>59</v>
@@ -4853,14 +4950,14 @@
       </c>
       <c r="O34" s="3"/>
       <c r="P34" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q34" s="2" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R34" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
@@ -4873,30 +4970,30 @@
     </row>
     <row r="35" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="B35" s="20"/>
       <c r="C35" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D35" s="20"/>
       <c r="E35" s="4" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="K35" s="4" t="s">
         <v>59</v>
@@ -4914,14 +5011,14 @@
       </c>
       <c r="O35" s="20"/>
       <c r="P35" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q35" s="4" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Lederansvar</v>
       </c>
       <c r="R35" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S35" s="20"/>
       <c r="T35" s="20"/>
@@ -4934,30 +5031,30 @@
     </row>
     <row r="36" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="2" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="K36" s="4" t="s">
         <v>59</v>
@@ -4975,14 +5072,14 @@
       </c>
       <c r="O36" s="3"/>
       <c r="P36" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q36" s="2" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Lederansvar</v>
       </c>
       <c r="R36" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
@@ -4995,30 +5092,30 @@
     </row>
     <row r="37" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="B37" s="20"/>
       <c r="C37" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="4" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="K37" s="4" t="s">
         <v>59</v>
@@ -5036,14 +5133,14 @@
       </c>
       <c r="O37" s="20"/>
       <c r="P37" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q37" s="4" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Lederansvar</v>
       </c>
       <c r="R37" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S37" s="20"/>
       <c r="T37" s="20"/>
@@ -5056,30 +5153,30 @@
     </row>
     <row r="38" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="2" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="K38" s="4" t="s">
         <v>59</v>
@@ -5097,14 +5194,14 @@
       </c>
       <c r="O38" s="3"/>
       <c r="P38" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q38" s="2" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Lederansvar</v>
       </c>
       <c r="R38" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
@@ -5117,30 +5214,30 @@
     </row>
     <row r="39" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="B39" s="20"/>
       <c r="C39" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D39" s="20"/>
       <c r="E39" s="4" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="K39" s="4" t="s">
         <v>59</v>
@@ -5158,14 +5255,14 @@
       </c>
       <c r="O39" s="20"/>
       <c r="P39" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q39" s="4" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Lederansvar</v>
       </c>
       <c r="R39" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S39" s="20"/>
       <c r="T39" s="20"/>
@@ -5178,30 +5275,30 @@
     </row>
     <row r="40" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="2" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="K40" s="4" t="s">
         <v>59</v>
@@ -5219,14 +5316,14 @@
       </c>
       <c r="O40" s="3"/>
       <c r="P40" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q40" s="2" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Lederansvar</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S40" s="3"/>
       <c r="T40" s="3"/>
@@ -5239,30 +5336,30 @@
     </row>
     <row r="41" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="B41" s="20"/>
       <c r="C41" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D41" s="20"/>
       <c r="E41" s="4" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>59</v>
@@ -5280,14 +5377,14 @@
       </c>
       <c r="O41" s="20"/>
       <c r="P41" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q41" s="4" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Lederansvar</v>
       </c>
       <c r="R41" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S41" s="20"/>
       <c r="T41" s="20"/>
@@ -5300,30 +5397,30 @@
     </row>
     <row r="42" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="2" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>59</v>
@@ -5341,14 +5438,14 @@
       </c>
       <c r="O42" s="3"/>
       <c r="P42" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q42" s="2" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Lederansvar</v>
       </c>
       <c r="R42" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
@@ -5361,30 +5458,30 @@
     </row>
     <row r="43" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="B43" s="20"/>
       <c r="C43" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="4" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>59</v>
@@ -5402,14 +5499,14 @@
       </c>
       <c r="O43" s="20"/>
       <c r="P43" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q43" s="4" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Lederansvar</v>
       </c>
       <c r="R43" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S43" s="20"/>
       <c r="T43" s="20"/>
@@ -5422,30 +5519,30 @@
     </row>
     <row r="44" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="2" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="K44" s="4" t="s">
         <v>59</v>
@@ -5463,14 +5560,14 @@
       </c>
       <c r="O44" s="3"/>
       <c r="P44" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q44" s="2" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Lederansvar</v>
       </c>
       <c r="R44" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
@@ -5483,30 +5580,30 @@
     </row>
     <row r="45" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="B45" s="20"/>
       <c r="C45" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="4" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="K45" s="4" t="s">
         <v>59</v>
@@ -5524,21 +5621,21 @@
       </c>
       <c r="O45" s="20"/>
       <c r="P45" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q45" s="4" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R45" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S45" s="4" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="T45" s="20"/>
       <c r="U45" s="4" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="V45" s="20"/>
       <c r="W45" s="20"/>
@@ -5548,30 +5645,30 @@
     </row>
     <row r="46" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="2" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="K46" s="4" t="s">
         <v>59</v>
@@ -5589,21 +5686,21 @@
       </c>
       <c r="O46" s="3"/>
       <c r="P46" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q46" s="2" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R46" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S46" s="2" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="T46" s="3"/>
       <c r="U46" s="2" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="V46" s="3"/>
       <c r="W46" s="3"/>
@@ -5613,30 +5710,30 @@
     </row>
     <row r="47" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="B47" s="20"/>
       <c r="C47" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="4" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="K47" s="4" t="s">
         <v>59</v>
@@ -5654,17 +5751,17 @@
       </c>
       <c r="O47" s="20"/>
       <c r="P47" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q47" s="4" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R47" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S47" s="4" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="T47" s="20"/>
       <c r="U47" s="20"/>
@@ -5676,30 +5773,30 @@
     </row>
     <row r="48" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="2" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="K48" s="4" t="s">
         <v>59</v>
@@ -5717,17 +5814,17 @@
       </c>
       <c r="O48" s="3"/>
       <c r="P48" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q48" s="2" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R48" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S48" s="2" t="s">
-        <v>271</v>
+        <v>279</v>
       </c>
       <c r="T48" s="3"/>
       <c r="U48" s="3"/>
@@ -5739,30 +5836,30 @@
     </row>
     <row r="49" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="B49" s="20"/>
       <c r="C49" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="4" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="K49" s="4" t="s">
         <v>59</v>
@@ -5780,21 +5877,21 @@
       </c>
       <c r="O49" s="20"/>
       <c r="P49" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q49" s="4" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R49" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S49" s="4" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="T49" s="20"/>
       <c r="U49" s="4" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="V49" s="20"/>
       <c r="W49" s="20"/>
@@ -5804,22 +5901,22 @@
     </row>
     <row r="50" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="2" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
       <c r="J50" s="2" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="K50" s="4" t="s">
         <v>59</v>
@@ -5837,21 +5934,21 @@
       </c>
       <c r="O50" s="3"/>
       <c r="P50" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q50" s="2" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R50" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S50" s="2" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="T50" s="3"/>
       <c r="U50" s="2" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="V50" s="3"/>
       <c r="W50" s="3"/>
@@ -5861,22 +5958,22 @@
     </row>
     <row r="51" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="B51" s="20"/>
       <c r="C51" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="4" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="F51" s="20"/>
       <c r="G51" s="20"/>
       <c r="H51" s="20"/>
       <c r="I51" s="20"/>
       <c r="J51" s="4" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="K51" s="4" t="s">
         <v>59</v>
@@ -5894,21 +5991,21 @@
       </c>
       <c r="O51" s="20"/>
       <c r="P51" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q51" s="4" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R51" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S51" s="4" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="T51" s="20"/>
       <c r="U51" s="4" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="V51" s="20"/>
       <c r="W51" s="20"/>
@@ -5918,22 +6015,22 @@
     </row>
     <row r="52" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="2" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
       <c r="J52" s="2" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="K52" s="4" t="s">
         <v>59</v>
@@ -5951,21 +6048,21 @@
       </c>
       <c r="O52" s="3"/>
       <c r="P52" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q52" s="2" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R52" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S52" s="2" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="T52" s="3"/>
       <c r="U52" s="2" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="V52" s="3"/>
       <c r="W52" s="3"/>
@@ -5975,22 +6072,22 @@
     </row>
     <row r="53" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="B53" s="20"/>
       <c r="C53" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D53" s="20"/>
       <c r="E53" s="4" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="F53" s="20"/>
       <c r="G53" s="20"/>
       <c r="H53" s="20"/>
       <c r="I53" s="20"/>
       <c r="J53" s="4" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="K53" s="4" t="s">
         <v>59</v>
@@ -6008,21 +6105,21 @@
       </c>
       <c r="O53" s="20"/>
       <c r="P53" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q53" s="4" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R53" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S53" s="4" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="T53" s="20"/>
       <c r="U53" s="4" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="V53" s="20"/>
       <c r="W53" s="20"/>
@@ -6032,22 +6129,22 @@
     </row>
     <row r="54" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="B54" s="3"/>
       <c r="C54" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" s="2" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
       <c r="J54" s="2" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="K54" s="4" t="s">
         <v>59</v>
@@ -6065,17 +6162,17 @@
       </c>
       <c r="O54" s="3"/>
       <c r="P54" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q54" s="2" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R54" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S54" s="2" t="s">
-        <v>271</v>
+        <v>279</v>
       </c>
       <c r="T54" s="3"/>
       <c r="U54" s="3" t="n">
@@ -6089,22 +6186,22 @@
     </row>
     <row r="55" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="B55" s="20"/>
       <c r="C55" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D55" s="20"/>
       <c r="E55" s="4" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="F55" s="20"/>
       <c r="G55" s="20"/>
       <c r="H55" s="20"/>
       <c r="I55" s="20"/>
       <c r="J55" s="4" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="K55" s="4" t="s">
         <v>59</v>
@@ -6122,21 +6219,21 @@
       </c>
       <c r="O55" s="20"/>
       <c r="P55" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q55" s="4" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R55" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S55" s="4" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="T55" s="20"/>
       <c r="U55" s="4" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="V55" s="20"/>
       <c r="W55" s="20"/>
@@ -6146,22 +6243,22 @@
     </row>
     <row r="56" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="2" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
       <c r="J56" s="2" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="K56" s="4" t="s">
         <v>59</v>
@@ -6179,21 +6276,21 @@
       </c>
       <c r="O56" s="3"/>
       <c r="P56" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q56" s="2" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R56" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S56" s="2" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="T56" s="3"/>
       <c r="U56" s="2" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="V56" s="3"/>
       <c r="W56" s="3"/>
@@ -6203,22 +6300,22 @@
     </row>
     <row r="57" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="B57" s="20"/>
       <c r="C57" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D57" s="20"/>
       <c r="E57" s="4" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="F57" s="20"/>
       <c r="G57" s="20"/>
       <c r="H57" s="20"/>
       <c r="I57" s="20"/>
       <c r="J57" s="4" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="K57" s="4" t="s">
         <v>59</v>
@@ -6236,21 +6333,21 @@
       </c>
       <c r="O57" s="20"/>
       <c r="P57" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="Q57" s="4" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R57" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="S57" s="4" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="T57" s="20"/>
       <c r="U57" s="4" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="V57" s="20"/>
       <c r="W57" s="20"/>
@@ -6261,7 +6358,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.3"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>

</xml_diff>

<commit_message>
Added more data to BALLERUP.xlsx
</commit_message>
<xml_diff>
--- a/tests/fixtures/BALLERUP.xlsx
+++ b/tests/fixtures/BALLERUP.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="bruger" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="321">
   <si>
     <t xml:space="preserve">operation</t>
   </si>
@@ -208,33 +208,36 @@
     <t xml:space="preserve">organisation</t>
   </si>
   <si>
+    <t xml:space="preserve">351fdf06-102a-4159-a5b4-69922b0ccde9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ee8dd627-9ff1-47c2-b900-aa3c214a31ee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7eadc1d9-19f5-46c7-a6db-f661c3a8fbb9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bestemmer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b4cd77e4-2ba0-47c7-93e9-22f7446abb57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noget</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tilknytning</t>
+  </si>
+  <si>
     <t xml:space="preserve">39dd14ed-faa9-40bf-9fc9-13c440078458</t>
   </si>
   <si>
-    <t xml:space="preserve">ee8dd627-9ff1-47c2-b900-aa3c214a31ee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7eadc1d9-19f5-46c7-a6db-f661c3a8fbb9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bestemmer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b4cd77e4-2ba0-47c7-93e9-22f7446abb57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Noget</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tilknytning</t>
-  </si>
-  <si>
     <t xml:space="preserve">f5b8f156-fa4e-46e2-b9e6-51a953166273</t>
   </si>
   <si>
@@ -250,6 +253,9 @@
     <t xml:space="preserve">Rolle</t>
   </si>
   <si>
+    <t xml:space="preserve">0838d00d-e2b3-4aa8-a5a5-649c2205ab21</t>
+  </si>
+  <si>
     <t xml:space="preserve">d82de46c-e266-4810-9e8d-e99a0c9c18d5</t>
   </si>
   <si>
@@ -262,6 +268,9 @@
     <t xml:space="preserve">Orlov</t>
   </si>
   <si>
+    <t xml:space="preserve">d7ec3a18-3a9d-43c8-ad03-0202c0d044d4</t>
+  </si>
+  <si>
     <t xml:space="preserve">brugerref_bvn</t>
   </si>
   <si>
@@ -397,6 +406,12 @@
     <t xml:space="preserve">Adressetype</t>
   </si>
   <si>
+    <t xml:space="preserve">d9aa489a-ac93-4769-98e5-19d6d37a919c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orlovstype</t>
+  </si>
+  <si>
     <t xml:space="preserve">titel</t>
   </si>
   <si>
@@ -445,9 +460,6 @@
     <t xml:space="preserve">Rettet</t>
   </si>
   <si>
-    <t xml:space="preserve">351fdf06-102a-4159-a5b4-69922b0ccde9</t>
-  </si>
-  <si>
     <t xml:space="preserve">d771715e-d0ad-48db-b12e-563ec9212df7</t>
   </si>
   <si>
@@ -971,6 +983,12 @@
   </si>
   <si>
     <t xml:space="preserve">Besvares indenfor to hverdage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barselsorlov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tillidsmand</t>
   </si>
 </sst>
 </file>
@@ -1218,6 +1236,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1227,10 +1249,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1258,24 +1276,24 @@
   <dimension ref="A1:M65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="S58:S59 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.3481781376518"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="4.2834008097166"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.8866396761134"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.0688259109312"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.21052631578947"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.96356275303644"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="32.8866396761134"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="33.4210526315789"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.7449392712551"/>
     <col collapsed="false" hidden="false" max="256" min="14" style="1" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.78542510121457"/>
   </cols>
@@ -1508,20 +1526,20 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="S58:S59 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.3481781376518"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.7773279352227"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.2105263157895"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.96356275303644"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.24696356275304"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.21052631578947"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="256" min="10" style="1" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.78542510121457"/>
   </cols>
@@ -1603,25 +1621,25 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+      <selection pane="topLeft" activeCell="N2" activeCellId="1" sqref="S58:S59 N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.1376518218623"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="4.17813765182186"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="2.25101214574899"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="2.03643724696356"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="32.3481781376518"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="1" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="1" width="32.7773279352227"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="1" width="8.24696356275304"/>
     <col collapsed="false" hidden="false" max="256" min="17" style="1" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.78542510121457"/>
@@ -1740,25 +1758,25 @@
   </sheetPr>
   <dimension ref="A1:M65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F59" activeCellId="1" sqref="S58:S59 F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="38.2429149797571"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="3.10526315789474"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="36.6356275303644"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="27.6356275303644"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.96356275303644"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="36.9554655870445"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="36.9554655870445"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="35.1336032388664"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="37.2793522267206"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="37.5991902834008"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="37.5991902834008"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="35.5627530364373"/>
     <col collapsed="false" hidden="false" max="256" min="14" style="1" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.57085020242915"/>
   </cols>
@@ -1830,7 +1848,7 @@
       <c r="I2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="21" t="s">
         <v>60</v>
       </c>
       <c r="K2" s="2" t="s">
@@ -1869,7 +1887,7 @@
       <c r="I3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="21" t="s">
         <v>60</v>
       </c>
       <c r="K3" s="2" t="s">
@@ -1907,7 +1925,7 @@
         <v>21</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>23</v>
@@ -1916,25 +1934,25 @@
         <v>40</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>58</v>
@@ -1946,7 +1964,7 @@
         <v>21</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>23</v>
@@ -1958,20 +1976,20 @@
     </row>
     <row r="6" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>58</v>
@@ -1983,7 +2001,7 @@
         <v>21</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>23</v>
@@ -1991,6 +2009,7 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
     </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2018,28 +2037,28 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
+      <selection pane="topLeft" activeCell="P1" activeCellId="1" sqref="S58:S59 P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="44.5627530364373"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.6356275303644"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="34.4939271255061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="43.919028340081"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="35.4574898785425"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="43.919028340081"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="34.919028340081"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="44.5627530364373"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="35.9919028340081"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="44.5627530364373"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="1" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="43.919028340081"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="44.5627530364373"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="1" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="13.1740890688259"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="1" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="256" min="20" style="1" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.78542510121457"/>
@@ -2062,63 +2081,63 @@
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B2" s="20"/>
       <c r="C2" s="16" t="n">
         <v>43115</v>
       </c>
-      <c r="D2" s="21"/>
+      <c r="D2" s="22"/>
       <c r="E2" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F2" s="20"/>
       <c r="G2" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>43</v>
@@ -2129,18 +2148,18 @@
       <c r="L2" s="4"/>
       <c r="M2" s="20"/>
       <c r="N2" s="4" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="O2" s="20"/>
       <c r="P2" s="4" t="s">
         <v>59</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="R2" s="20"/>
       <c r="S2" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2306,29 +2325,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="1" sqref="S58:S59 A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="38.0283400809717"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="38.668016194332"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.46153846153846"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="3.10526315789474"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="37.919028340081"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="37.919028340081"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="38.5627530364372"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="36.9554655870445"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="37.5991902834008"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="10.2834008097166"/>
     <col collapsed="false" hidden="false" max="253" min="16" style="1" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="1025" min="254" style="0" width="8.57085020242915"/>
   </cols>
@@ -2350,39 +2369,39 @@
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B2" s="20"/>
       <c r="C2" s="16" t="n">
@@ -2390,7 +2409,7 @@
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="4" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F2" s="20"/>
       <c r="G2" s="4" t="s">
@@ -2414,23 +2433,23 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="22" t="n">
+      <c r="C3" s="23" t="n">
         <v>43115</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="4" t="s">
@@ -2454,15 +2473,15 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B4" s="20"/>
       <c r="C4" s="16" t="n">
@@ -2470,7 +2489,7 @@
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="4" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F4" s="20"/>
       <c r="G4" s="4" t="s">
@@ -2494,23 +2513,23 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="22" t="n">
+      <c r="C5" s="23" t="n">
         <v>43115</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="4" t="s">
@@ -2534,15 +2553,15 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="16" t="n">
@@ -2550,7 +2569,7 @@
       </c>
       <c r="D6" s="20"/>
       <c r="E6" s="4" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F6" s="20"/>
       <c r="G6" s="4" t="s">
@@ -2574,23 +2593,23 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="22" t="n">
+      <c r="C7" s="23" t="n">
         <v>43115</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="4" t="s">
@@ -2614,15 +2633,15 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="16" t="n">
@@ -2630,9 +2649,9 @@
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F8" s="23"/>
+        <v>117</v>
+      </c>
+      <c r="F8" s="24"/>
       <c r="G8" s="4" t="s">
         <v>59</v>
       </c>
@@ -2654,25 +2673,25 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="24" t="s">
-        <v>115</v>
+      <c r="A9" s="21" t="s">
+        <v>118</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="16" t="n">
         <v>43115</v>
       </c>
       <c r="D9" s="20"/>
-      <c r="E9" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="F9" s="23"/>
+      <c r="E9" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="F9" s="24"/>
       <c r="G9" s="4" t="s">
         <v>59</v>
       </c>
@@ -2694,23 +2713,23 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="C10" s="22" t="n">
+      <c r="C10" s="23" t="n">
         <v>43115</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F10" s="25"/>
       <c r="G10" s="4" t="s">
@@ -2734,15 +2753,15 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="16" t="n">
@@ -2750,9 +2769,9 @@
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="F11" s="23"/>
+        <v>123</v>
+      </c>
+      <c r="F11" s="24"/>
       <c r="G11" s="4" t="s">
         <v>59</v>
       </c>
@@ -2774,23 +2793,23 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B12" s="3"/>
-      <c r="C12" s="22" t="n">
+      <c r="C12" s="23" t="n">
         <v>43115</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="4" t="s">
@@ -2814,10 +2833,50 @@
         <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="23" t="n">
+        <v>43115</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F13" s="25"/>
+      <c r="G13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="4" t="str">
+        <f aca="false">organisation!$A$2</f>
+        <v>3a87187c-f25a-40a1-8d42-312b2e2b43bd</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K13" s="2" t="str">
+        <f aca="false">organisation!$A$2</f>
+        <v>3a87187c-f25a-40a1-8d42-312b2e2b43bd</v>
+      </c>
+      <c r="L13" s="3"/>
+      <c r="M13" s="2" t="str">
+        <f aca="false">klassifikation!$A$2</f>
+        <v>439936fe-4c4c-49a4-827b-70f9e50f8486</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2836,41 +2895,41 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z57"/>
+  <dimension ref="A1:Z59"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="5" topLeftCell="J6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
+      <selection pane="bottomLeft" activeCell="S58" activeCellId="0" sqref="S58:S59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="36.2064777327935"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="36.8502024291498"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="3"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="34.3846153846154"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="28.3846153846154"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="34.8137651821862"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="27.9595141700405"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="34.3846153846154"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="35.4574898785425"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="34.8137651821862"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="35.2429149797571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="28.3846153846154"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="34.8137651821862"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="35.9919028340081"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="1" width="11.246963562753"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="35.4574898785425"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="35.9919028340081"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="1" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.1781376518219"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="9.63967611336032"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="9.85425101214575"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="1" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="26.8866396761134"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="34.7085020242915"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="27.3157894736842"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="35.1336032388664"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="19.4939271255061"/>
     <col collapsed="false" hidden="false" max="24" min="24" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="10.2834008097166"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="1" width="13.8178137651822"/>
     <col collapsed="false" hidden="false" max="255" min="27" style="1" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="1025" min="256" style="0" width="8.57085020242915"/>
@@ -2893,95 +2952,95 @@
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="U1" s="2" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B2" s="20"/>
       <c r="C2" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="4" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>59</v>
@@ -2999,14 +3058,14 @@
       </c>
       <c r="O2" s="20"/>
       <c r="P2" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q2" s="4" t="str">
         <f aca="false">facet!$E$8</f>
         <v>Tilknytningstype</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S2" s="20"/>
       <c r="T2" s="20"/>
@@ -3018,31 +3077,31 @@
       <c r="Z2" s="20"/>
     </row>
     <row r="3" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="s">
-        <v>139</v>
+      <c r="A3" s="21" t="s">
+        <v>60</v>
       </c>
       <c r="B3" s="20"/>
       <c r="C3" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D3" s="20"/>
       <c r="E3" s="4" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>59</v>
@@ -3060,13 +3119,13 @@
       </c>
       <c r="O3" s="20"/>
       <c r="P3" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S3" s="20"/>
       <c r="T3" s="20"/>
@@ -3078,31 +3137,31 @@
       <c r="Z3" s="20"/>
     </row>
     <row r="4" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="s">
-        <v>140</v>
+      <c r="A4" s="21" t="s">
+        <v>144</v>
       </c>
       <c r="B4" s="20"/>
       <c r="C4" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>136</v>
-      </c>
       <c r="H4" s="4" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>59</v>
@@ -3120,13 +3179,13 @@
       </c>
       <c r="O4" s="20"/>
       <c r="P4" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S4" s="20"/>
       <c r="T4" s="20"/>
@@ -3138,31 +3197,31 @@
       <c r="Z4" s="20"/>
     </row>
     <row r="5" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="24" t="s">
-        <v>142</v>
+      <c r="A5" s="21" t="s">
+        <v>146</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D5" s="20"/>
       <c r="E5" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>138</v>
-      </c>
       <c r="J5" s="4" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>59</v>
@@ -3180,13 +3239,13 @@
       </c>
       <c r="O5" s="20"/>
       <c r="P5" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S5" s="20"/>
       <c r="T5" s="20"/>
@@ -3203,26 +3262,26 @@
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>59</v>
@@ -3240,14 +3299,14 @@
       </c>
       <c r="O6" s="3"/>
       <c r="P6" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q6" s="2" t="str">
         <f aca="false">facet!$E$7</f>
         <v>Stillingsbetegnelse</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
@@ -3260,30 +3319,30 @@
     </row>
     <row r="7" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="4" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>59</v>
@@ -3301,14 +3360,14 @@
       </c>
       <c r="O7" s="20"/>
       <c r="P7" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q7" s="4" t="str">
         <f aca="false">facet!$E$7</f>
         <v>Stillingsbetegnelse</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S7" s="20"/>
       <c r="T7" s="20"/>
@@ -3321,30 +3380,30 @@
     </row>
     <row r="8" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="2" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>59</v>
@@ -3362,14 +3421,14 @@
       </c>
       <c r="O8" s="3"/>
       <c r="P8" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q8" s="2" t="str">
         <f aca="false">facet!$E$7</f>
         <v>Stillingsbetegnelse</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
@@ -3382,30 +3441,30 @@
     </row>
     <row r="9" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="4" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>59</v>
@@ -3423,14 +3482,14 @@
       </c>
       <c r="O9" s="20"/>
       <c r="P9" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q9" s="4" t="str">
         <f aca="false">facet!$E$7</f>
         <v>Stillingsbetegnelse</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S9" s="20"/>
       <c r="T9" s="20"/>
@@ -3443,30 +3502,30 @@
     </row>
     <row r="10" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="2" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>59</v>
@@ -3484,14 +3543,14 @@
       </c>
       <c r="O10" s="3"/>
       <c r="P10" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q10" s="2" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
@@ -3504,30 +3563,30 @@
     </row>
     <row r="11" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="4" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>59</v>
@@ -3545,14 +3604,14 @@
       </c>
       <c r="O11" s="20"/>
       <c r="P11" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q11" s="4" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S11" s="20"/>
       <c r="T11" s="20"/>
@@ -3565,27 +3624,27 @@
     </row>
     <row r="12" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>31</v>
@@ -3606,18 +3665,18 @@
       </c>
       <c r="O12" s="3"/>
       <c r="P12" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q12" s="2" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S12" s="3"/>
       <c r="T12" s="2" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
@@ -3628,30 +3687,30 @@
     </row>
     <row r="13" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B13" s="20"/>
       <c r="C13" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="4" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>59</v>
@@ -3669,14 +3728,14 @@
       </c>
       <c r="O13" s="20"/>
       <c r="P13" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q13" s="4" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S13" s="20"/>
       <c r="T13" s="20"/>
@@ -3689,30 +3748,30 @@
     </row>
     <row r="14" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="2" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>59</v>
@@ -3730,14 +3789,14 @@
       </c>
       <c r="O14" s="3"/>
       <c r="P14" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q14" s="2" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
@@ -3750,30 +3809,30 @@
     </row>
     <row r="15" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B15" s="20"/>
       <c r="C15" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="4" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>59</v>
@@ -3791,14 +3850,14 @@
       </c>
       <c r="O15" s="20"/>
       <c r="P15" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q15" s="4" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S15" s="20"/>
       <c r="T15" s="20"/>
@@ -3811,30 +3870,30 @@
     </row>
     <row r="16" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="2" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>59</v>
@@ -3852,14 +3911,14 @@
       </c>
       <c r="O16" s="3"/>
       <c r="P16" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q16" s="2" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
@@ -3872,30 +3931,30 @@
     </row>
     <row r="17" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B17" s="20"/>
       <c r="C17" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="4" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>59</v>
@@ -3913,14 +3972,14 @@
       </c>
       <c r="O17" s="20"/>
       <c r="P17" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q17" s="4" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R17" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S17" s="20"/>
       <c r="T17" s="20"/>
@@ -3933,30 +3992,30 @@
     </row>
     <row r="18" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="2" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>59</v>
@@ -3974,14 +4033,14 @@
       </c>
       <c r="O18" s="3"/>
       <c r="P18" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q18" s="2" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
@@ -3994,30 +4053,30 @@
     </row>
     <row r="19" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B19" s="20"/>
       <c r="C19" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="4" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>59</v>
@@ -4035,14 +4094,14 @@
       </c>
       <c r="O19" s="20"/>
       <c r="P19" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q19" s="4" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R19" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S19" s="20"/>
       <c r="T19" s="20"/>
@@ -4055,30 +4114,30 @@
     </row>
     <row r="20" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="2" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="K20" s="4" t="s">
         <v>59</v>
@@ -4096,14 +4155,14 @@
       </c>
       <c r="O20" s="3"/>
       <c r="P20" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q20" s="2" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
@@ -4116,30 +4175,30 @@
     </row>
     <row r="21" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B21" s="20"/>
       <c r="C21" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="4" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="K21" s="4" t="s">
         <v>59</v>
@@ -4157,14 +4216,14 @@
       </c>
       <c r="O21" s="20"/>
       <c r="P21" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q21" s="4" t="str">
         <f aca="false">facet!$E$5</f>
         <v>Enhedstype</v>
       </c>
       <c r="R21" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S21" s="20"/>
       <c r="T21" s="20"/>
@@ -4177,30 +4236,30 @@
     </row>
     <row r="22" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="2" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="K22" s="4" t="s">
         <v>59</v>
@@ -4218,14 +4277,14 @@
       </c>
       <c r="O22" s="3"/>
       <c r="P22" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q22" s="2" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
@@ -4238,30 +4297,30 @@
     </row>
     <row r="23" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B23" s="20"/>
       <c r="C23" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="4" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="K23" s="4" t="s">
         <v>59</v>
@@ -4279,14 +4338,14 @@
       </c>
       <c r="O23" s="20"/>
       <c r="P23" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q23" s="4" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R23" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S23" s="20"/>
       <c r="T23" s="20"/>
@@ -4299,30 +4358,30 @@
     </row>
     <row r="24" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="2" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="K24" s="4" t="s">
         <v>59</v>
@@ -4340,14 +4399,14 @@
       </c>
       <c r="O24" s="3"/>
       <c r="P24" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q24" s="2" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
@@ -4360,30 +4419,30 @@
     </row>
     <row r="25" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B25" s="20"/>
       <c r="C25" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="4" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="K25" s="4" t="s">
         <v>59</v>
@@ -4401,14 +4460,14 @@
       </c>
       <c r="O25" s="20"/>
       <c r="P25" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q25" s="4" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R25" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S25" s="20"/>
       <c r="T25" s="20"/>
@@ -4421,30 +4480,30 @@
     </row>
     <row r="26" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="2" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="K26" s="4" t="s">
         <v>59</v>
@@ -4462,14 +4521,14 @@
       </c>
       <c r="O26" s="3"/>
       <c r="P26" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q26" s="2" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
@@ -4482,30 +4541,30 @@
     </row>
     <row r="27" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B27" s="20"/>
       <c r="C27" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="4" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="K27" s="4" t="s">
         <v>59</v>
@@ -4523,14 +4582,14 @@
       </c>
       <c r="O27" s="20"/>
       <c r="P27" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q27" s="4" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R27" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S27" s="20"/>
       <c r="T27" s="20"/>
@@ -4543,30 +4602,30 @@
     </row>
     <row r="28" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="2" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="K28" s="4" t="s">
         <v>59</v>
@@ -4584,14 +4643,14 @@
       </c>
       <c r="O28" s="3"/>
       <c r="P28" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q28" s="2" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
@@ -4604,30 +4663,30 @@
     </row>
     <row r="29" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B29" s="20"/>
       <c r="C29" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="4" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="K29" s="4" t="s">
         <v>59</v>
@@ -4645,14 +4704,14 @@
       </c>
       <c r="O29" s="20"/>
       <c r="P29" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q29" s="4" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R29" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S29" s="20"/>
       <c r="T29" s="20"/>
@@ -4665,30 +4724,30 @@
     </row>
     <row r="30" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="2" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="K30" s="4" t="s">
         <v>59</v>
@@ -4706,14 +4765,14 @@
       </c>
       <c r="O30" s="3"/>
       <c r="P30" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q30" s="2" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R30" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
@@ -4726,30 +4785,30 @@
     </row>
     <row r="31" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B31" s="20"/>
       <c r="C31" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D31" s="20"/>
       <c r="E31" s="4" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="K31" s="4" t="s">
         <v>59</v>
@@ -4767,14 +4826,14 @@
       </c>
       <c r="O31" s="20"/>
       <c r="P31" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q31" s="4" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R31" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S31" s="20"/>
       <c r="T31" s="20"/>
@@ -4787,30 +4846,30 @@
     </row>
     <row r="32" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="2" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="K32" s="4" t="s">
         <v>59</v>
@@ -4828,14 +4887,14 @@
       </c>
       <c r="O32" s="3"/>
       <c r="P32" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q32" s="2" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
@@ -4848,30 +4907,30 @@
     </row>
     <row r="33" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B33" s="20"/>
       <c r="C33" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D33" s="20"/>
       <c r="E33" s="4" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="K33" s="4" t="s">
         <v>59</v>
@@ -4889,14 +4948,14 @@
       </c>
       <c r="O33" s="20"/>
       <c r="P33" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q33" s="4" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R33" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S33" s="20"/>
       <c r="T33" s="20"/>
@@ -4909,30 +4968,30 @@
     </row>
     <row r="34" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="2" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="K34" s="4" t="s">
         <v>59</v>
@@ -4950,14 +5009,14 @@
       </c>
       <c r="O34" s="3"/>
       <c r="P34" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q34" s="2" t="str">
         <f aca="false">facet!$E$10</f>
         <v>Ledertyper</v>
       </c>
       <c r="R34" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
@@ -4970,30 +5029,30 @@
     </row>
     <row r="35" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B35" s="20"/>
       <c r="C35" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D35" s="20"/>
       <c r="E35" s="4" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="K35" s="4" t="s">
         <v>59</v>
@@ -5011,14 +5070,14 @@
       </c>
       <c r="O35" s="20"/>
       <c r="P35" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q35" s="4" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Lederansvar</v>
       </c>
       <c r="R35" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S35" s="20"/>
       <c r="T35" s="20"/>
@@ -5031,30 +5090,30 @@
     </row>
     <row r="36" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="2" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="K36" s="4" t="s">
         <v>59</v>
@@ -5072,14 +5131,14 @@
       </c>
       <c r="O36" s="3"/>
       <c r="P36" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q36" s="2" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Lederansvar</v>
       </c>
       <c r="R36" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
@@ -5092,30 +5151,30 @@
     </row>
     <row r="37" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B37" s="20"/>
       <c r="C37" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="4" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="K37" s="4" t="s">
         <v>59</v>
@@ -5133,14 +5192,14 @@
       </c>
       <c r="O37" s="20"/>
       <c r="P37" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q37" s="4" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Lederansvar</v>
       </c>
       <c r="R37" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S37" s="20"/>
       <c r="T37" s="20"/>
@@ -5153,30 +5212,30 @@
     </row>
     <row r="38" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="2" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="K38" s="4" t="s">
         <v>59</v>
@@ -5194,14 +5253,14 @@
       </c>
       <c r="O38" s="3"/>
       <c r="P38" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q38" s="2" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Lederansvar</v>
       </c>
       <c r="R38" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
@@ -5214,30 +5273,30 @@
     </row>
     <row r="39" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B39" s="20"/>
       <c r="C39" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D39" s="20"/>
       <c r="E39" s="4" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="K39" s="4" t="s">
         <v>59</v>
@@ -5255,14 +5314,14 @@
       </c>
       <c r="O39" s="20"/>
       <c r="P39" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q39" s="4" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Lederansvar</v>
       </c>
       <c r="R39" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S39" s="20"/>
       <c r="T39" s="20"/>
@@ -5275,30 +5334,30 @@
     </row>
     <row r="40" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="2" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="K40" s="4" t="s">
         <v>59</v>
@@ -5316,14 +5375,14 @@
       </c>
       <c r="O40" s="3"/>
       <c r="P40" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q40" s="2" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Lederansvar</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S40" s="3"/>
       <c r="T40" s="3"/>
@@ -5336,30 +5395,30 @@
     </row>
     <row r="41" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="B41" s="20"/>
       <c r="C41" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D41" s="20"/>
       <c r="E41" s="4" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>59</v>
@@ -5377,14 +5436,14 @@
       </c>
       <c r="O41" s="20"/>
       <c r="P41" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q41" s="4" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Lederansvar</v>
       </c>
       <c r="R41" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S41" s="20"/>
       <c r="T41" s="20"/>
@@ -5397,30 +5456,30 @@
     </row>
     <row r="42" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="2" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>59</v>
@@ -5438,14 +5497,14 @@
       </c>
       <c r="O42" s="3"/>
       <c r="P42" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q42" s="2" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Lederansvar</v>
       </c>
       <c r="R42" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
@@ -5458,30 +5517,30 @@
     </row>
     <row r="43" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B43" s="20"/>
       <c r="C43" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="4" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>59</v>
@@ -5499,14 +5558,14 @@
       </c>
       <c r="O43" s="20"/>
       <c r="P43" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q43" s="4" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Lederansvar</v>
       </c>
       <c r="R43" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S43" s="20"/>
       <c r="T43" s="20"/>
@@ -5519,30 +5578,30 @@
     </row>
     <row r="44" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="2" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="K44" s="4" t="s">
         <v>59</v>
@@ -5560,14 +5619,14 @@
       </c>
       <c r="O44" s="3"/>
       <c r="P44" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q44" s="2" t="str">
         <f aca="false">facet!$E$11</f>
         <v>Lederansvar</v>
       </c>
       <c r="R44" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
@@ -5580,30 +5639,30 @@
     </row>
     <row r="45" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="B45" s="20"/>
       <c r="C45" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="4" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="K45" s="4" t="s">
         <v>59</v>
@@ -5621,21 +5680,21 @@
       </c>
       <c r="O45" s="20"/>
       <c r="P45" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q45" s="4" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R45" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S45" s="4" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="T45" s="20"/>
       <c r="U45" s="4" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="V45" s="20"/>
       <c r="W45" s="20"/>
@@ -5645,30 +5704,30 @@
     </row>
     <row r="46" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="2" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="K46" s="4" t="s">
         <v>59</v>
@@ -5686,21 +5745,21 @@
       </c>
       <c r="O46" s="3"/>
       <c r="P46" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q46" s="2" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R46" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S46" s="2" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="T46" s="3"/>
       <c r="U46" s="2" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="V46" s="3"/>
       <c r="W46" s="3"/>
@@ -5710,30 +5769,30 @@
     </row>
     <row r="47" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="B47" s="20"/>
       <c r="C47" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="4" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="K47" s="4" t="s">
         <v>59</v>
@@ -5751,17 +5810,17 @@
       </c>
       <c r="O47" s="20"/>
       <c r="P47" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q47" s="4" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R47" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S47" s="4" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="T47" s="20"/>
       <c r="U47" s="20"/>
@@ -5773,30 +5832,30 @@
     </row>
     <row r="48" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="2" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="K48" s="4" t="s">
         <v>59</v>
@@ -5814,17 +5873,17 @@
       </c>
       <c r="O48" s="3"/>
       <c r="P48" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q48" s="2" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R48" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S48" s="2" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="T48" s="3"/>
       <c r="U48" s="3"/>
@@ -5836,30 +5895,30 @@
     </row>
     <row r="49" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="B49" s="20"/>
       <c r="C49" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="4" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="K49" s="4" t="s">
         <v>59</v>
@@ -5877,21 +5936,21 @@
       </c>
       <c r="O49" s="20"/>
       <c r="P49" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q49" s="4" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R49" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S49" s="4" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="T49" s="20"/>
       <c r="U49" s="4" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="V49" s="20"/>
       <c r="W49" s="20"/>
@@ -5901,22 +5960,22 @@
     </row>
     <row r="50" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="2" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
       <c r="J50" s="2" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="K50" s="4" t="s">
         <v>59</v>
@@ -5934,21 +5993,21 @@
       </c>
       <c r="O50" s="3"/>
       <c r="P50" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q50" s="2" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R50" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S50" s="2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="T50" s="3"/>
       <c r="U50" s="2" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="V50" s="3"/>
       <c r="W50" s="3"/>
@@ -5958,22 +6017,22 @@
     </row>
     <row r="51" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="B51" s="20"/>
       <c r="C51" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="4" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="F51" s="20"/>
       <c r="G51" s="20"/>
       <c r="H51" s="20"/>
       <c r="I51" s="20"/>
       <c r="J51" s="4" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="K51" s="4" t="s">
         <v>59</v>
@@ -5991,21 +6050,21 @@
       </c>
       <c r="O51" s="20"/>
       <c r="P51" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q51" s="4" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R51" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S51" s="4" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="T51" s="20"/>
       <c r="U51" s="4" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="V51" s="20"/>
       <c r="W51" s="20"/>
@@ -6015,22 +6074,22 @@
     </row>
     <row r="52" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="2" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
       <c r="J52" s="2" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="K52" s="4" t="s">
         <v>59</v>
@@ -6048,21 +6107,21 @@
       </c>
       <c r="O52" s="3"/>
       <c r="P52" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q52" s="2" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R52" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S52" s="2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="T52" s="3"/>
       <c r="U52" s="2" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="V52" s="3"/>
       <c r="W52" s="3"/>
@@ -6072,22 +6131,22 @@
     </row>
     <row r="53" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="B53" s="20"/>
       <c r="C53" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D53" s="20"/>
       <c r="E53" s="4" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="F53" s="20"/>
       <c r="G53" s="20"/>
       <c r="H53" s="20"/>
       <c r="I53" s="20"/>
       <c r="J53" s="4" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="K53" s="4" t="s">
         <v>59</v>
@@ -6105,21 +6164,21 @@
       </c>
       <c r="O53" s="20"/>
       <c r="P53" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q53" s="4" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R53" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S53" s="4" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="T53" s="20"/>
       <c r="U53" s="4" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="V53" s="20"/>
       <c r="W53" s="20"/>
@@ -6129,22 +6188,22 @@
     </row>
     <row r="54" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="B54" s="3"/>
       <c r="C54" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" s="2" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
       <c r="J54" s="2" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="K54" s="4" t="s">
         <v>59</v>
@@ -6162,17 +6221,17 @@
       </c>
       <c r="O54" s="3"/>
       <c r="P54" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q54" s="2" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R54" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S54" s="2" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="T54" s="3"/>
       <c r="U54" s="3" t="n">
@@ -6186,22 +6245,22 @@
     </row>
     <row r="55" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="B55" s="20"/>
       <c r="C55" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D55" s="20"/>
       <c r="E55" s="4" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="F55" s="20"/>
       <c r="G55" s="20"/>
       <c r="H55" s="20"/>
       <c r="I55" s="20"/>
       <c r="J55" s="4" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="K55" s="4" t="s">
         <v>59</v>
@@ -6219,21 +6278,21 @@
       </c>
       <c r="O55" s="20"/>
       <c r="P55" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q55" s="4" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R55" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S55" s="4" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="T55" s="20"/>
       <c r="U55" s="4" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="V55" s="20"/>
       <c r="W55" s="20"/>
@@ -6243,22 +6302,22 @@
     </row>
     <row r="56" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="2" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
       <c r="J56" s="2" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="K56" s="4" t="s">
         <v>59</v>
@@ -6276,21 +6335,21 @@
       </c>
       <c r="O56" s="3"/>
       <c r="P56" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q56" s="2" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R56" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S56" s="2" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="T56" s="3"/>
       <c r="U56" s="2" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="V56" s="3"/>
       <c r="W56" s="3"/>
@@ -6300,22 +6359,22 @@
     </row>
     <row r="57" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="B57" s="20"/>
       <c r="C57" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D57" s="20"/>
       <c r="E57" s="4" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="F57" s="20"/>
       <c r="G57" s="20"/>
       <c r="H57" s="20"/>
       <c r="I57" s="20"/>
       <c r="J57" s="4" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="K57" s="4" t="s">
         <v>59</v>
@@ -6333,27 +6392,131 @@
       </c>
       <c r="O57" s="20"/>
       <c r="P57" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q57" s="4" t="str">
         <f aca="false">facet!$E$12</f>
         <v>Adressetype</v>
       </c>
       <c r="R57" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S57" s="4" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="T57" s="20"/>
       <c r="U57" s="4" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="V57" s="20"/>
       <c r="W57" s="20"/>
       <c r="X57" s="20"/>
       <c r="Y57" s="20"/>
       <c r="Z57" s="20"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B58" s="20"/>
+      <c r="C58" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D58" s="20"/>
+      <c r="E58" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="F58" s="20"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="20"/>
+      <c r="I58" s="20"/>
+      <c r="J58" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="K58" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="L58" s="4" t="str">
+        <f aca="false">organisation!$A$2</f>
+        <v>3a87187c-f25a-40a1-8d42-312b2e2b43bd</v>
+      </c>
+      <c r="M58" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N58" s="4" t="str">
+        <f aca="false">organisation!$A$2</f>
+        <v>3a87187c-f25a-40a1-8d42-312b2e2b43bd</v>
+      </c>
+      <c r="O58" s="20"/>
+      <c r="P58" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q58" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="R58" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="S58" s="4"/>
+      <c r="T58" s="20"/>
+      <c r="U58" s="4"/>
+      <c r="V58" s="20"/>
+      <c r="W58" s="20"/>
+      <c r="X58" s="20"/>
+      <c r="Y58" s="20"/>
+      <c r="Z58" s="20"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B59" s="20"/>
+      <c r="C59" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D59" s="20"/>
+      <c r="E59" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="F59" s="20"/>
+      <c r="G59" s="20"/>
+      <c r="H59" s="20"/>
+      <c r="I59" s="20"/>
+      <c r="J59" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="K59" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="L59" s="4" t="str">
+        <f aca="false">organisation!$A$2</f>
+        <v>3a87187c-f25a-40a1-8d42-312b2e2b43bd</v>
+      </c>
+      <c r="M59" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N59" s="4" t="str">
+        <f aca="false">organisation!$A$2</f>
+        <v>3a87187c-f25a-40a1-8d42-312b2e2b43bd</v>
+      </c>
+      <c r="O59" s="20"/>
+      <c r="P59" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q59" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="R59" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="S59" s="4"/>
+      <c r="T59" s="20"/>
+      <c r="U59" s="4"/>
+      <c r="V59" s="20"/>
+      <c r="W59" s="20"/>
+      <c r="X59" s="20"/>
+      <c r="Y59" s="20"/>
+      <c r="Z59" s="20"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
BALLERUP: add IT systems
</commit_message>
<xml_diff>
--- a/tests/fixtures/BALLERUP.xlsx
+++ b/tests/fixtures/BALLERUP.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="bruger" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,6 +15,7 @@
     <sheet name="klassifikation" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="facet" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="klasse" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="itsystem" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="333">
   <si>
     <t xml:space="preserve">operation</t>
   </si>
@@ -989,21 +990,56 @@
   </si>
   <si>
     <t xml:space="preserve">Tillidsmand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">itsystemnavn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">itsystemtype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">konfigurationreference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tilhoerer_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tilknyttedeorganisationer_bvn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a7ecd46a-9d70-4170-bde9-9bf44cf8632b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2010-01-01 00:00:00+01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active Directory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">990255f7-44c7-4fec-9ef8-27fe73763afd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LoRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lokal Rammearkitektur</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0"/>
-    <numFmt numFmtId="167" formatCode="YYYY/MM/DD"/>
-    <numFmt numFmtId="168" formatCode="YYYY/DD/MM"/>
-    <numFmt numFmtId="169" formatCode="####"/>
+    <numFmt numFmtId="167" formatCode="YYYY/DD/MM"/>
+    <numFmt numFmtId="168" formatCode="####"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1039,6 +1075,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1054,7 +1096,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="15">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1125,6 +1167,41 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1151,7 +1228,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1240,19 +1317,47 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1273,29 +1378,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M65536"/>
+  <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="S58:S59 D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="M3 D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.4"/>
+  <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.3481781376518"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="4.2834008097166"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.21052631578947"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.1781376518219"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="33.4210526315789"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="256" min="14" style="1" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.78542510121457"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="33.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="8.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="15.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="14" style="1" width="8.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1510,7 +1615,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1525,23 +1630,23 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="S58:S59 A2"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="M3 C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.4"/>
+  <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.7773279352227"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.96356275303644"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.21052631578947"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="256" min="10" style="1" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.78542510121457"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="10" style="1" width="8.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1605,7 +1710,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
@@ -1620,29 +1725,29 @@
   </sheetPr>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="1" sqref="S58:S59 N2"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N2" activeCellId="1" sqref="M3 N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.4"/>
+  <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.1376518218623"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="4.17813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="2.03643724696356"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="32.3481781376518"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.21052631578947"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="1" width="32.7773279352227"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="256" min="17" style="1" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.78542510121457"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="4.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="2.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="32.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="15.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="1" width="32.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="8.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="17" style="1" width="8.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1743,7 +1848,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
@@ -1756,29 +1861,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M65536"/>
+  <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F59" activeCellId="1" sqref="S58:S59 F59"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="1" sqref="M3 G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.4"/>
+  <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="38.2429149797571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="3.10526315789474"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="37.2793522267206"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="28.0647773279352"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.1781376518219"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="37.5991902834008"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="37.5991902834008"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="35.5627530364373"/>
-    <col collapsed="false" hidden="false" max="256" min="14" style="1" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="3.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="37.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="28.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="37.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="37.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="35.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="14" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2021,7 +2126,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2036,32 +2141,32 @@
   </sheetPr>
   <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P1" activeCellId="1" sqref="S58:S59 P1"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P1" activeCellId="1" sqref="M3 P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.4"/>
+  <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="44.5627530364373"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.6356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="34.919028340081"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="44.5627530364373"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="35.9919028340081"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="44.5627530364373"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="44.5627530364373"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="9.21052631578947"/>
-    <col collapsed="false" hidden="false" max="256" min="20" style="1" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.78542510121457"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="34.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="20.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="44.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="35.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="44.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="44.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="9.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="20" style="1" width="8.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2131,7 +2236,7 @@
       <c r="C2" s="16" t="n">
         <v>43115</v>
       </c>
-      <c r="D2" s="22"/>
+      <c r="D2" s="16"/>
       <c r="E2" s="4" t="s">
         <v>96</v>
       </c>
@@ -2312,7 +2417,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.3"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
@@ -2327,29 +2432,29 @@
   </sheetPr>
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="1" sqref="S58:S59 A13"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="1" sqref="M3 A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.4"/>
+  <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="38.668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.46153846153846"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="3.10526315789474"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="38.5627530364372"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="38.5627530364372"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="37.5991902834008"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="253" min="16" style="1" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="1025" min="254" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.46"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="3.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="38.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="12.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="38.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="8.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="37.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="10.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="253" min="16" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="254" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2444,7 +2549,7 @@
         <v>106</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="23" t="n">
+      <c r="C3" s="22" t="n">
         <v>43115</v>
       </c>
       <c r="D3" s="3"/>
@@ -2524,7 +2629,7 @@
         <v>110</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="23" t="n">
+      <c r="C5" s="22" t="n">
         <v>43115</v>
       </c>
       <c r="D5" s="3"/>
@@ -2604,7 +2709,7 @@
         <v>114</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="23" t="n">
+      <c r="C7" s="22" t="n">
         <v>43115</v>
       </c>
       <c r="D7" s="3"/>
@@ -2651,7 +2756,7 @@
       <c r="E8" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="F8" s="24"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="4" t="s">
         <v>59</v>
       </c>
@@ -2691,7 +2796,7 @@
       <c r="E9" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="F9" s="24"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="4" t="s">
         <v>59</v>
       </c>
@@ -2724,14 +2829,14 @@
         <v>120</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="C10" s="23" t="n">
+      <c r="C10" s="22" t="n">
         <v>43115</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F10" s="25"/>
+      <c r="F10" s="24"/>
       <c r="G10" s="4" t="s">
         <v>59</v>
       </c>
@@ -2771,7 +2876,7 @@
       <c r="E11" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="F11" s="24"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="4" t="s">
         <v>59</v>
       </c>
@@ -2804,14 +2909,14 @@
         <v>124</v>
       </c>
       <c r="B12" s="3"/>
-      <c r="C12" s="23" t="n">
+      <c r="C12" s="22" t="n">
         <v>43115</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F12" s="25"/>
+      <c r="F12" s="24"/>
       <c r="G12" s="4" t="s">
         <v>59</v>
       </c>
@@ -2844,14 +2949,14 @@
         <v>126</v>
       </c>
       <c r="B13" s="3"/>
-      <c r="C13" s="23" t="n">
+      <c r="C13" s="22" t="n">
         <v>43115</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F13" s="25"/>
+      <c r="F13" s="24"/>
       <c r="G13" s="4" t="s">
         <v>59</v>
       </c>
@@ -2882,7 +2987,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.3"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
@@ -2897,42 +3002,42 @@
   </sheetPr>
   <dimension ref="A1:Z59"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="5" topLeftCell="J6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
-      <selection pane="bottomLeft" activeCell="S58" activeCellId="0" sqref="S58:S59"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="J2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="O12" activeCellId="1" sqref="M3 O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.4"/>
+  <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="36.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="3"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="34.8137651821862"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="35.2429149797571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="28.3846153846154"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="34.8137651821862"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="35.9919028340081"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="11.246963562753"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="35.9919028340081"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="9.85425101214575"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="27.3157894736842"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="35.1336032388664"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="255" min="27" style="1" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="1025" min="256" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="2.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="28.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="35.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="28.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="34.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="13.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="35.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="35.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="8.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="27.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="35.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="13.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="10.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="13.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="27" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="256" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6521,10 +6626,254 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.3"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M3" activeCellId="0" sqref="M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="39.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="5.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="22.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="25" width="7.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="25" width="17.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="25" width="21.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="25" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="25" width="20.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="25" width="38.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="25" width="16.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="25" width="22.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="25" width="26.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="25" width="9.64"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="251" min="14" style="25" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>321</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26" t="s">
+        <v>328</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>329</v>
+      </c>
+      <c r="G2" s="26"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28" t="s">
+        <v>331</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>332</v>
+      </c>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="30"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="30"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="30"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="30"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="30"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="30"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="31"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="32"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
BALLERUP: use correct organisation UUID
</commit_message>
<xml_diff>
--- a/tests/fixtures/BALLERUP.xlsx
+++ b/tests/fixtures/BALLERUP.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="bruger" sheetId="1" state="visible" r:id="rId2"/>
@@ -1381,7 +1381,7 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="M3 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1630,8 +1630,8 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="M3 C2"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1726,7 +1726,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="1" sqref="M3 N2"/>
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="1" sqref="M3 G4"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2142,7 +2142,7 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P1" activeCellId="1" sqref="M3 P1"/>
+      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2433,7 +2433,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="1" sqref="M3 A13"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3005,7 +3005,7 @@
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="J2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="O12" activeCellId="1" sqref="M3 O12"/>
+      <selection pane="bottomLeft" activeCell="O12" activeCellId="0" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6641,8 +6641,8 @@
   </sheetPr>
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M3" activeCellId="0" sqref="M3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6722,7 +6722,7 @@
       <c r="G2" s="26"/>
       <c r="H2" s="27"/>
       <c r="I2" s="2" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="J2" s="26" t="s">
         <v>59</v>
@@ -6751,7 +6751,7 @@
       <c r="G3" s="28"/>
       <c r="H3" s="28"/>
       <c r="I3" s="2" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="J3" s="26" t="s">
         <v>59</v>

</xml_diff>